<commit_message>
Arreglado el error causado por el ID de iframe dinámico
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,120 +456,384 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Huawei Freebuds 5i</t>
+          <t>Nothing Ear (2)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>69.90000000000001</v>
+        <v>135</v>
       </c>
       <c r="C2" t="n">
-        <v>78.84999999999999</v>
+        <v>146.15</v>
       </c>
       <c r="D2" t="n">
-        <v>12.80400572246064</v>
+        <v>8.259259259259263</v>
       </c>
       <c r="E2" t="n">
-        <v>8.949999999999989</v>
+        <v>11.15000000000001</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202282533_-freebuds-5i-huawei.html</t>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202568190_-ear-2-nothing-tech.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bose Headphones 700</t>
+          <t>Huawei Freebuds 5i</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>238.93</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>249.99</v>
+        <v>78</v>
       </c>
       <c r="D3" t="n">
-        <v>4.628970828276064</v>
+        <v>9.704641350210979</v>
       </c>
       <c r="E3" t="n">
-        <v>11.06</v>
+        <v>6.900000000000006</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/6594549_-headphones-700-bose.html</t>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202282533_-freebuds-5i-huawei.html</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apple EarPods</t>
+          <t>LG TONE Free DFP8</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11.49</v>
+        <v>59.4</v>
       </c>
       <c r="C4" t="n">
-        <v>16.49</v>
+        <v>69</v>
       </c>
       <c r="D4" t="n">
-        <v>43.5161009573542</v>
+        <v>16.16161616161617</v>
       </c>
       <c r="E4" t="n">
-        <v>4.999999999999998</v>
+        <v>9.600000000000001</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/3533650_-earpods-apple.html</t>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201653276_-tone-free-dfp8-lg-electronics.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Samsung Galaxy Buds 2 Pro SM-R510</t>
+          <t>Apple iPhone 6S</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>137.99</v>
+        <v>119.95</v>
       </c>
       <c r="C5" t="n">
-        <v>146.99</v>
+        <v>248.08</v>
       </c>
       <c r="D5" t="n">
-        <v>6.522211754474962</v>
+        <v>106.8195081283868</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>128.13</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202054804_-galaxy-buds-2-pro-sm-r510-bora-purple-samsung.html</t>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/4842805_-iphone-6s-apple.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JBL Tune 720BT</t>
+          <t>Bowers &amp; Wilkins PX7 S2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51.12</v>
+        <v>199</v>
       </c>
       <c r="C6" t="n">
-        <v>64.98999999999999</v>
+        <v>428.37</v>
       </c>
       <c r="D6" t="n">
-        <v>27.13223787167449</v>
+        <v>115.2613065326633</v>
       </c>
       <c r="E6" t="n">
-        <v>13.87</v>
+        <v>229.37</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202496304_-tune-720bt-jbl-audio.html</t>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202011022_-px7-s2-schwarz-bowers-wilkins.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sony WH-1000XM5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>296.57</v>
+      </c>
+      <c r="C7" t="n">
+        <v>299</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8193681087095818</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.430000000000007</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201952086_-wh-1000xm5-black-sony.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sony WH-1000XM4</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>249.05</v>
+      </c>
+      <c r="C8" t="n">
+        <v>269.99</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8.407950210801042</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20.94</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/200278050_-wh-1000xm4-schwarz-sony.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>JBL Wave 200TWS</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>42.77</v>
+      </c>
+      <c r="C9" t="n">
+        <v>52.48</v>
+      </c>
+      <c r="D9" t="n">
+        <v>22.70282908580779</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9.709999999999994</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201746578_-wave-200tws-jbl-audio.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sony WH-CH720N</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>79.98999999999999</v>
+      </c>
+      <c r="C10" t="n">
+        <v>86.98</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.738592324040518</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6.990000000000009</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202334761_-wh-ch720n-sony.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sony LinkBuds S</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>129</v>
+      </c>
+      <c r="C11" t="n">
+        <v>146</v>
+      </c>
+      <c r="D11" t="n">
+        <v>13.17829457364341</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201961566_-linkbuds-s-schwarz-sony.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Marshall Major IV</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>79.98999999999999</v>
+      </c>
+      <c r="C12" t="n">
+        <v>129.9</v>
+      </c>
+      <c r="D12" t="n">
+        <v>62.39529941242657</v>
+      </c>
+      <c r="E12" t="n">
+        <v>49.91000000000001</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/200799717_-major-iv-marshall.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LG TONE Free DFP9E</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>76.48999999999999</v>
+      </c>
+      <c r="C13" t="n">
+        <v>84.98999999999999</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11.11256373382142</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202056848_-tone-free-dfp9e-lg-electronics.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Buds 2 Pro SM-R510</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>139.9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>169.09</v>
+      </c>
+      <c r="D14" t="n">
+        <v>20.86490350250178</v>
+      </c>
+      <c r="E14" t="n">
+        <v>29.19</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202054812_-galaxy-buds-2-pro-sm-r510-white-samsung.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Skullcandy Crusher Evo</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>122.8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>144.99</v>
+      </c>
+      <c r="D15" t="n">
+        <v>18.07003257328991</v>
+      </c>
+      <c r="E15" t="n">
+        <v>22.19000000000001</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/200818290_-crusher-evo-skullcandy.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Beats By Dre Studio3 Wireless</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>197.91</v>
+      </c>
+      <c r="C16" t="n">
+        <v>269</v>
+      </c>
+      <c r="D16" t="n">
+        <v>35.92036784396948</v>
+      </c>
+      <c r="E16" t="n">
+        <v>71.09</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/5760160_-studio3-wireless-beats-by-dr-dre.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Xiaomi Buds 3T Pro</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>35.99</v>
+      </c>
+      <c r="C17" t="n">
+        <v>54.43</v>
+      </c>
+      <c r="D17" t="n">
+        <v>51.23645457071407</v>
+      </c>
+      <c r="E17" t="n">
+        <v>18.44</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201838960_-buds-3t-pro-xiaomi.html</t>
         </is>
       </c>
     </row>

</xml_diff>